<commit_message>
aún siguen sin andar edit y form
</commit_message>
<xml_diff>
--- a/traspaso a seeder de deliverables.xlsx
+++ b/traspaso a seeder de deliverables.xlsx
@@ -351,7 +351,29 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -363,7 +385,12 @@
       </fill>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -661,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F103" sqref="F2:F103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -671,6 +698,10 @@
       <c r="D1" t="s">
         <v>0</v>
       </c>
+      <c r="F1" t="str">
+        <f>CONCATENATE("'",A1,"' =&gt; '",B1,"','",C1,"' =&gt; '",E1,"',")</f>
+        <v>'' =&gt; '','' =&gt; '',</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3020,7 +3051,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>